<commit_message>
Update: New tests implemented
</commit_message>
<xml_diff>
--- a/ConnectorDescriptor_test_plan.xlsx
+++ b/ConnectorDescriptor_test_plan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristi\PycharmProjects\AssemblyConnector\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000" activeTab="1"/>
   </bookViews>
@@ -13,9 +18,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Overview!$A$1:$E$23</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
   <si>
     <t>Requirements</t>
   </si>
@@ -216,6 +221,18 @@
     <t>- check that the connector is created between the Rport and the Pport who is referencing the &lt;AswcDiagForDcm&gt;</t>
   </si>
   <si>
+    <t>- check that one connector is created, between the Pport and the Rport</t>
+  </si>
+  <si>
+    <t>Check that the tool will not generate an existing connector</t>
+  </si>
+  <si>
+    <t>- check that no connector is created between the Rport and the Pport</t>
+  </si>
+  <si>
+    <t>Check that for unique Pport and Rport, only one connector will be created</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -235,8 +252,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: feed to the tool one Rport referencing an ASWC_Data and two Pport, one of the Pport referencing &lt;AswcDiagForDcm&gt;, while the other one is referencing another ASWC</t>
-    </r>
+      <t>: feed to the tool one Pport referencing one interface of type Client-Server, one Rport referencing the same interface as the Pport, and one connector which already contains the link between the given ports</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that only one connector is created between the given ports</t>
+  </si>
+  <si>
+    <t>Check that the tool will not discriminate between Pports and PRPorts</t>
   </si>
   <si>
     <r>
@@ -248,24 +271,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Test 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one Rport referencing an ASWC_Data, and one Pport referencing the same interface as the Rport, but from &lt;AswcDiagForDcm&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Check that the tool generate the correct connectors when having multiple Rports with the same name and referencing the same interface </t>
-  </si>
-  <si>
-    <t>Check that the tool generate the correct connectors when Pport and Rport references the same interface</t>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one PPort referencing one interface of type Client-Server and one Rport referencing the same Client-Server interface</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that one connector is created between the PRPort and the Rport</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - check in the log that all the input .arxml files are parsed</t>
   </si>
   <si>
     <r>
@@ -287,151 +313,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: feed to the tool one Pport referencing one interface of type Client-Server, and two Rports with the same short-name as the Pport and  referencing the same interface as the Pport</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one Pport referencing one interface of type Client-Server, and  one Rport with a different short-name as of Pport, but referencing the same interface as the PPort</t>
-    </r>
-  </si>
-  <si>
-    <t>- check that two connectors are created, one for each Rport</t>
-  </si>
-  <si>
-    <t>- check that one connector is created, between the Pport and the Rport</t>
-  </si>
-  <si>
-    <t>Check that the tool will not generate an existing connector</t>
-  </si>
-  <si>
-    <t>- check that no connector is created between the Rport and the Pport</t>
-  </si>
-  <si>
-    <t>Check that for unique Pport and Rport, only one connector will be created</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one Pport referencing one interface of type Client-Server, one Rport referencing the same interface as the Pport, and one connector which already contains the link between the given ports</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one Port referencing one interface of type Client-Server and one Rport referencing the same Client-Server interface</t>
-    </r>
-  </si>
-  <si>
-    <t>- check that only one connector is created between the given ports</t>
-  </si>
-  <si>
-    <t>Check that the tool will not discriminate between Pports and PRPorts</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one PPort referencing one interface of type Client-Server and one Rport referencing the same Client-Server interface</t>
-    </r>
-  </si>
-  <si>
-    <t>- check that one connector is created between the PRPort and the Rport</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - check in the log that all the input .arxml files are parsed</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>: provide to the tool several .arxml  files as an input argument</t>
     </r>
   </si>
@@ -439,53 +320,7 @@
     <t>n/a</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one Port referencing one interface of type Client-Server and one Rport referencing the same Client-Server interface</t>
-    </r>
-  </si>
-  <si>
     <t>-check that the output file does not contains multiple times the same connector</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: feed to the tool one PRPort referencing one interface of type Client-Server, and one Rport referencing the samei Client-Server interface</t>
-    </r>
   </si>
   <si>
     <t>Implemented</t>
@@ -531,9 +366,6 @@
     <t>TRS.CONNECTOR.FUNC.0006</t>
   </si>
   <si>
-    <t>TRS.CONNECTOR.FUNC.0009</t>
-  </si>
-  <si>
     <t>TRS.CONNECTOR.GEN.001</t>
   </si>
   <si>
@@ -584,12 +416,6 @@
     <t>TRS.CONNECTOR.FUNC.010</t>
   </si>
   <si>
-    <t>TRS.CONNECTOR.FUNC.011</t>
-  </si>
-  <si>
-    <t>TRS.CONNECTOR.FUNC.012</t>
-  </si>
-  <si>
     <t>Covered by TRS.CONNECTOR.CHECK.003 and TRS.CONNECTOR.CHECK.004</t>
   </si>
   <si>
@@ -605,6 +431,48 @@
     <t>Check that the tool does not generate the output file in case of any error present</t>
   </si>
   <si>
+    <t>- check that the connector is created between the Pport and the Rport</t>
+  </si>
+  <si>
+    <t>4/18/2018</t>
+  </si>
+  <si>
+    <t>CHECK.ARXML</t>
+  </si>
+  <si>
+    <t>- check that the error isn't present in the log file</t>
+  </si>
+  <si>
+    <t>- check the log for the corresponding error</t>
+  </si>
+  <si>
+    <t>Check the tool behavior for each case when there are different COREs/PARTITIONs or they're not different</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test 3: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>feed to the tool an input file which contains two Pport referencing the same interface and having different short-names (eg: SR_name and 123_name), and one Rport referencing the same interface referenced by the Pport</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that a connector is created in the output file for both Pports.</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.CHECK.001</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.CHECK.002</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -614,6 +482,113 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Test 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provide to the tool  one Rport  referencing  one interface of type CLIENT-SERVER-INTERFACE, one file which contains two Pports referencing the same interface as the Rport and having the same short-name, and one 'xml' file which contains the same Cores and Partitions allocation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provide to the tool  one Rport  referencing  one interface of type CLIENT-SERVER-INTERFACE, one file which contains two Pports referencing the same interface as the Rport and having the same short-name, and one 'xml' file which contains different Cores and Partitions allocation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one PRPort referencing one interface of type Client-Server, and one Rport referencing the same Client-Server interface</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one PPort referencing one interface of type Client-Server and one Rport referencing the same Client-Server interface</t>
+    </r>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.007</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.008</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.FUNC.009</t>
+  </si>
+  <si>
+    <t>TRS.CONNECTOR.GEN.003</t>
+  </si>
+  <si>
+    <t>Check that the tool generate the correct connectors when an unique Pport and an unique Rport references the same interface</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Test 1</t>
     </r>
     <r>
@@ -624,6 +599,109 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>: feed to the tool one PPort referencing one interface of type Client-Server, and  one RPort with a different short-name as of PPort, but referencing the same interface as the PPort</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one Pport referencing one interface of type Client-Server, and two RPorts with different names as the PPort and  referencing the same interface as the Rports, and having the same names</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that two connectors are created, for each pair of (Pport, RPort) with the same name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that the tool generate the correct connectors when having multiple Rports and Pports with the same name and referencing the same interface </t>
+  </si>
+  <si>
+    <t>Check that the tool makes the differnce when dealing with Pports from &lt;Aswc_IntDcm&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one Rport referencing an ASWC_Data and two Pport, one of the Pport referencing &lt;Aswc_IntDcm&gt;, while the other one is referencing another ASWC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: feed to the tool one Rport referencing an ASWC_Data, and one Pport referencing the same interface as the Rport, but from &lt;Aswc_IntDcm&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>: feed to the tool one Rport referencing a MODE-SWITHC-INTERFACE and one Pport referencing the same interface, but where the SHORT-NAME has not any of the above forms</t>
     </r>
   </si>
@@ -637,6 +715,50 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: feed to the tool one Rport referencing a MODE-SWITCH-INTERFACE and one Pport referencing the same interface, where the SHORT-NAME of the Pport being of form </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BswM_ModeSwitchPort_&lt;OS_APP_NAME_BSWM&gt;_Switch_Rte_&lt;CORE&gt;_&lt;PARTITION&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, where the CORE and PARTITION are the same with the ones used by the RPort</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Test 2</t>
     </r>
     <r>
@@ -647,13 +769,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: feed to the tool one Rport referencing a MODE-SWITCH-INTERFACE and one Pport referencing the same interface, where the SHORT-NAME of the Pport being of form OsApp_&lt;CORE&gt;_&lt;PARTITION&gt;_BswMSwitchLocalPort , where the CORE and PARTITION are the same with the ones used by the RPort</t>
-    </r>
-  </si>
-  <si>
-    <t>Check that the tool makes the differnce when dealing with Pports from &lt;AswcDiagForDcm&gt;</t>
-  </si>
-  <si>
+      <t xml:space="preserve">: feed to the tool one Rport referencing a MODE-SWITCH-INTERFACE and one Pport referencing the same interface, where the SHORT-NAME of the Pport being of form </t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -663,6 +780,38 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>BswM_ModeSwitchPort_&lt;OS_APP_NAME_BSWM&gt;_Switch_Rte_&lt;CORE&gt;_&lt;PARTITION&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, where the CORE and PARTITION are not the same with the ones used by the RPort</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that no connection is created between the Pport and the Rport</t>
+  </si>
+  <si>
+    <t>Check that the tool correctly evaluates the SHORT-NAME of an port</t>
+  </si>
+  <si>
+    <t>- check that the connector is created between the two given ports</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Test 1</t>
     </r>
     <r>
@@ -673,97 +822,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: feed to the tool one Rport referencing a MODE-SWITCH-INTERFACE and one Pport referencing the same interface, where the SHORT-NAME of the Pport being of form OsApp_&lt;CORE&gt;_&lt;PARTITION&gt;_AppSwitchLocalPort , where the CORE and PARTITION are the same with the ones used by the RPort</t>
-    </r>
-  </si>
-  <si>
-    <t>- check that the connector is created between the Pport and the Rport</t>
-  </si>
-  <si>
-    <t>4/18/2018</t>
-  </si>
-  <si>
-    <t>CHECK.ARXML</t>
-  </si>
-  <si>
-    <t>- check that the error isn't present in the log file</t>
-  </si>
-  <si>
-    <t>- check the log for the corresponding error</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 4:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Provide to the tool  one Rport  referencing  one interface of type CLIENT-SERVER-INTERFACE, one file which contains two Pports referencing the same interface as the Rport and having the same short-name, and one 'xml' file which contains the same Cores and Partitions allocation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 5:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Provide to the tool  one Rport  referencing  one interface of type CLIENT-SERVER-INTERFACE, one file which contains two Pports referencing the same interface as the Rport and having the same short-name, and one 'xml' file which contains different Cores and Partitions allocation</t>
-    </r>
-  </si>
-  <si>
-    <t>Check the tool behavior for each case when there are different COREs/PARTITIONs or they're not different</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Test 3: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>feed to the tool an input file which contains two Pport referencing the same interface and having different short-names (eg: SR_name and 123_name), and one Rport referencing the same interface referenced by the Pport</t>
-    </r>
-  </si>
-  <si>
-    <t>- check that a connector is created in the output file for both Pports.</t>
+      <t>: provide to the tool one Rport referencing an interface which has the name of format &lt;RP_xyz&gt;, and one Pport referencing the same interface which has the format &lt;xyz&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,6 +840,49 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1154,7 +1264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1245,6 +1355,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1257,73 +1412,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1386,6 +1497,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1416,21 +1537,41 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1722,154 +1863,154 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="68.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
@@ -1882,17 +2023,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" style="18" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" style="1" customWidth="1"/>
@@ -1902,7 +2043,7 @@
     <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1915,210 +2056,210 @@
       <c r="D1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="49" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30.75" thickTop="1">
+      <c r="E1" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="51" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="20" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30">
-      <c r="A5" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>37</v>
+      <c r="F4" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>29</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D5" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="54"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30">
-      <c r="A6" s="39"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30">
-      <c r="A7" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="D7" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="54"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30">
-      <c r="A8" s="39"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>45</v>
-      </c>
       <c r="E8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45">
+      <c r="F8" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45">
-      <c r="A10" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>26</v>
+      <c r="F9" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="58" t="s">
+        <v>90</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45">
-      <c r="A11" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>25</v>
+      <c r="F10" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="58" t="s">
+        <v>94</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45">
-      <c r="A12" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>87</v>
+      <c r="F11" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="54" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>95</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>21</v>
@@ -2126,15 +2267,15 @@
       <c r="E12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45">
-      <c r="A13" s="39"/>
-      <c r="B13" s="38"/>
+      <c r="F12" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="54"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="19" t="s">
-        <v>24</v>
+        <v>97</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>22</v>
@@ -2142,89 +2283,89 @@
       <c r="E13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="60">
-      <c r="A14" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>82</v>
+      <c r="F13" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>69</v>
       </c>
       <c r="C14" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="54"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="60">
-      <c r="A15" s="39"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="45">
-      <c r="A16" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>89</v>
+      <c r="B16" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="60" t="s">
+        <v>72</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30">
+      <c r="F16" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30">
+      <c r="F17" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B18" s="35" t="s">
         <v>4</v>
@@ -2238,13 +2379,13 @@
       <c r="E18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="30">
+      <c r="F18" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>8</v>
@@ -2258,15 +2399,15 @@
       <c r="E19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="60">
-      <c r="A20" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="40" t="s">
+      <c r="F19" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="55" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -2278,13 +2419,13 @@
       <c r="E20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="60">
-      <c r="A21" s="39"/>
-      <c r="B21" s="40"/>
+      <c r="F20" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="54"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="19" t="s">
         <v>16</v>
       </c>
@@ -2294,155 +2435,176 @@
       <c r="E21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45">
-      <c r="A22" s="39"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="53" t="s">
-        <v>97</v>
+      <c r="F21" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="54"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="45" t="s">
+        <v>78</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45">
-      <c r="A23" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="40" t="s">
+      <c r="F22" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="55" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45">
-      <c r="A24" s="48"/>
-      <c r="B24" s="40"/>
+      <c r="F23" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="51"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="45">
-      <c r="A25" s="48"/>
-      <c r="B25" s="40"/>
+      <c r="F24" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="52"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="19" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="60">
-      <c r="A26" s="48"/>
-      <c r="B26" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="51" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="60">
-      <c r="A27" s="45"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>92</v>
+      <c r="F25" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>76</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="51" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30.75" thickBot="1">
-      <c r="A29" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="55" t="s">
-        <v>40</v>
+      <c r="F27" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="52"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="47" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E23"/>
-  <mergeCells count="13">
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A23:A27"/>
+  <mergeCells count="14">
+    <mergeCell ref="B27:B28"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B23:B25"/>
@@ -2454,41 +2616,43 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A23:A25"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28 F2:F25">
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
+  <conditionalFormatting sqref="F29 F2:F26">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F29">
-    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
+  <conditionalFormatting sqref="F2:F30">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29 F26:F27">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+  <conditionalFormatting sqref="F30 F27:F28">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:F27 F29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F27:F28 F30">
       <formula1>"YES, NO, N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E30">
       <formula1>"done, not done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28 F2:F25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F29 F2:F26">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>